<commit_message>
Upload : SQL Query for Owner
</commit_message>
<xml_diff>
--- a/Documents/Specification/Database_Specification.xlsx
+++ b/Documents/Specification/Database_Specification.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="92">
   <si>
     <t>회원정보</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -244,9 +244,6 @@
   <si>
     <t>answer_date</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>owner_id</t>
   </si>
   <si>
     <t>rs_id</t>
@@ -769,7 +766,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -777,7 +774,7 @@
     <col min="1" max="15" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,14 +783,13 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -805,18 +801,15 @@
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -827,14 +820,11 @@
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -844,9 +834,9 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
@@ -861,10 +851,10 @@
         <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -884,7 +874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -893,10 +883,10 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
@@ -908,7 +898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -925,7 +915,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -938,7 +928,7 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>18</v>
@@ -990,10 +980,10 @@
         <v>51</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>23</v>
@@ -1034,7 +1024,7 @@
         <v>27</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1049,13 +1039,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>52</v>
@@ -1101,13 +1091,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>35</v>
@@ -1122,7 +1112,7 @@
         <v>33</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -1148,7 +1138,7 @@
         <v>33</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -1165,13 +1155,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>30</v>
@@ -1180,13 +1170,13 @@
         <v>48</v>
       </c>
       <c r="F36" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="H36" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -1206,13 +1196,13 @@
         <v>48</v>
       </c>
       <c r="F37" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="H37" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -1226,13 +1216,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>41</v>
@@ -1268,13 +1258,13 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>49</v>
@@ -1296,7 +1286,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1307,25 +1297,25 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="D49" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="F49" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -1339,16 +1329,16 @@
         <v>48</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E50" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>